<commit_message>
added code to write on sheet, also modified defect details
Added code to write on sheet, also modified defect details, based on
month and then count for monthly defect data is also created
</commit_message>
<xml_diff>
--- a/examples/Defect.xlsx
+++ b/examples/Defect.xlsx
@@ -2,34 +2,26 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\python study\web crawler\Python_webcrawler\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$B$41</definedName>
-  </definedNames>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="81">
   <si>
     <t>defect ID</t>
   </si>
@@ -37,91 +29,241 @@
     <t>date</t>
   </si>
   <si>
+    <t>priority</t>
+  </si>
+  <si>
+    <t>Sprint 1</t>
+  </si>
+  <si>
+    <t>Sprint 2</t>
+  </si>
+  <si>
+    <t>Sprint 4</t>
+  </si>
+  <si>
+    <t>Sprint 5</t>
+  </si>
+  <si>
+    <t>Sprint 6</t>
+  </si>
+  <si>
+    <t>Sprint 7</t>
+  </si>
+  <si>
+    <t>Sprint 8</t>
+  </si>
+  <si>
+    <t>Sprint 9</t>
+  </si>
+  <si>
+    <t>Sprint 10</t>
+  </si>
+  <si>
+    <t>Sprint 11</t>
+  </si>
+  <si>
+    <t>Sprint 14</t>
+  </si>
+  <si>
+    <t>Sprint 15</t>
+  </si>
+  <si>
+    <t>Sprint 16</t>
+  </si>
+  <si>
+    <t>Sprint 17</t>
+  </si>
+  <si>
+    <t>Sprint 18</t>
+  </si>
+  <si>
+    <t>Sprint 20</t>
+  </si>
+  <si>
+    <t>Sprint 22</t>
+  </si>
+  <si>
+    <t>Sprint 23</t>
+  </si>
+  <si>
+    <t>Sprint 25</t>
+  </si>
+  <si>
     <t>Sprint date</t>
   </si>
   <si>
-    <t>Sprint 1</t>
-  </si>
-  <si>
-    <t>Sprint 2</t>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>End Date</t>
   </si>
   <si>
     <t>Sprint 3</t>
   </si>
   <si>
-    <t>Sprint 4</t>
-  </si>
-  <si>
-    <t>Start Date</t>
-  </si>
-  <si>
-    <t>End Date</t>
-  </si>
-  <si>
-    <t>priority</t>
-  </si>
-  <si>
-    <t>Sprint 5</t>
-  </si>
-  <si>
-    <t>Sprint 6</t>
-  </si>
-  <si>
-    <t>Sprint 7</t>
-  </si>
-  <si>
-    <t>Sprint 8</t>
-  </si>
-  <si>
-    <t>Sprint 9</t>
-  </si>
-  <si>
-    <t>Sprint 10</t>
-  </si>
-  <si>
-    <t>Sprint 11</t>
-  </si>
-  <si>
     <t>Sprint 12</t>
   </si>
   <si>
     <t>Sprint 13</t>
   </si>
   <si>
-    <t>Sprint 14</t>
-  </si>
-  <si>
-    <t>Sprint 15</t>
-  </si>
-  <si>
-    <t>Sprint 16</t>
-  </si>
-  <si>
-    <t>Sprint 17</t>
-  </si>
-  <si>
-    <t>Sprint 18</t>
-  </si>
-  <si>
     <t>Sprint 19</t>
   </si>
   <si>
-    <t>Sprint 20</t>
-  </si>
-  <si>
     <t>Sprint 21</t>
   </si>
   <si>
-    <t>Sprint 22</t>
-  </si>
-  <si>
-    <t>Sprint 23</t>
-  </si>
-  <si>
     <t>Sprint 24</t>
   </si>
   <si>
-    <t>Sprint 25</t>
+    <t>2015-01-01 00:00:00</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>January 2015</t>
+  </si>
+  <si>
+    <t>2015-01-03 00:00:00</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>2015-01-06 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-01-10 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-01-16 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-01-17 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-02-18 00:00:00</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>February 2015</t>
+  </si>
+  <si>
+    <t>2015-02-20 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-03-03 00:00:00</t>
+  </si>
+  <si>
+    <t>March 2015</t>
+  </si>
+  <si>
+    <t>2015-03-07 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-03-09 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-03-17 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-04-05 00:00:00</t>
+  </si>
+  <si>
+    <t>April 2015</t>
+  </si>
+  <si>
+    <t>2015-04-15 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-04-25 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-05-09 00:00:00</t>
+  </si>
+  <si>
+    <t>May 2015</t>
+  </si>
+  <si>
+    <t>2015-05-14 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-05-19 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-05-21 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-06-01 00:00:00</t>
+  </si>
+  <si>
+    <t>June 2015</t>
+  </si>
+  <si>
+    <t>2015-06-05 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-07-15 00:00:00</t>
+  </si>
+  <si>
+    <t>July 2015</t>
+  </si>
+  <si>
+    <t>2015-07-25 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-08-08 00:00:00</t>
+  </si>
+  <si>
+    <t>August 2015</t>
+  </si>
+  <si>
+    <t>2015-08-19 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-08-20 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-09-02 00:00:00</t>
+  </si>
+  <si>
+    <t>September 2015</t>
+  </si>
+  <si>
+    <t>2015-09-25 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-09-27 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-10-24 00:00:00</t>
+  </si>
+  <si>
+    <t>October 2015</t>
+  </si>
+  <si>
+    <t>2015-10-25 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-11-12 00:00:00</t>
+  </si>
+  <si>
+    <t>November 2015</t>
+  </si>
+  <si>
+    <t>2015-11-21 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-12-11 00:00:00</t>
+  </si>
+  <si>
+    <t>December 2015</t>
+  </si>
+  <si>
+    <t>2015-12-30 00:00:00</t>
   </si>
 </sst>
 </file>
@@ -171,7 +313,9 @@
   <dxfs count="1">
     <dxf>
       <font>
+        <sz val="11"/>
         <color rgb="FF9C0006"/>
+        <name val="Calibri"/>
       </font>
       <fill>
         <patternFill>
@@ -180,7 +324,7 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -457,11 +601,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D2" sqref="A2:D5"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
@@ -475,7 +619,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -573,7 +717,7 @@
         <v>3</v>
       </c>
       <c r="D8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -587,7 +731,7 @@
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -601,7 +745,7 @@
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -615,7 +759,7 @@
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -629,7 +773,7 @@
         <v>3</v>
       </c>
       <c r="D12" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -643,7 +787,7 @@
         <v>3</v>
       </c>
       <c r="D13" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -657,7 +801,7 @@
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -671,7 +815,7 @@
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -685,7 +829,7 @@
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -699,7 +843,7 @@
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -713,7 +857,7 @@
         <v>2</v>
       </c>
       <c r="D18" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -727,7 +871,7 @@
         <v>3</v>
       </c>
       <c r="D19" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -741,7 +885,7 @@
         <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -755,7 +899,7 @@
         <v>3</v>
       </c>
       <c r="D21" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -769,7 +913,7 @@
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -783,7 +927,7 @@
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -797,7 +941,7 @@
         <v>2</v>
       </c>
       <c r="D24" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -811,7 +955,7 @@
         <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -825,7 +969,7 @@
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -839,7 +983,7 @@
         <v>3</v>
       </c>
       <c r="D27" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -853,7 +997,7 @@
         <v>2</v>
       </c>
       <c r="D28" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -867,7 +1011,7 @@
         <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -881,7 +1025,7 @@
         <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -895,7 +1039,7 @@
         <v>1</v>
       </c>
       <c r="D31" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -909,7 +1053,7 @@
         <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -923,7 +1067,7 @@
         <v>1</v>
       </c>
       <c r="D33" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -937,7 +1081,7 @@
         <v>2</v>
       </c>
       <c r="D34" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -951,7 +1095,7 @@
         <v>2</v>
       </c>
       <c r="D35" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -965,7 +1109,7 @@
         <v>2</v>
       </c>
       <c r="D36" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -979,7 +1123,7 @@
         <v>2</v>
       </c>
       <c r="D37" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -993,7 +1137,7 @@
         <v>3</v>
       </c>
       <c r="D38" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1007,7 +1151,7 @@
         <v>3</v>
       </c>
       <c r="D39" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1021,7 +1165,7 @@
         <v>1</v>
       </c>
       <c r="D40" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1035,15 +1179,12 @@
         <v>1</v>
       </c>
       <c r="D41" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:C42">
-    <sortCondition ref="B2:B42"/>
-  </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
@@ -1055,7 +1196,7 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
@@ -1065,13 +1206,13 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1102,7 +1243,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B4" s="2">
         <v>42035</v>
@@ -1115,7 +1256,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="2">
         <v>42050</v>
@@ -1128,7 +1269,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B6" s="2">
         <v>42065</v>
@@ -1141,7 +1282,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B7" s="2">
         <v>42080</v>
@@ -1154,7 +1295,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B8" s="2">
         <v>42095</v>
@@ -1167,7 +1308,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B9" s="2">
         <v>42110</v>
@@ -1180,7 +1321,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B10" s="2">
         <v>42125</v>
@@ -1193,7 +1334,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B11" s="2">
         <v>42140</v>
@@ -1206,7 +1347,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B12" s="2">
         <v>42155</v>
@@ -1219,7 +1360,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B13" s="2">
         <v>42170</v>
@@ -1232,7 +1373,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B14" s="2">
         <v>42185</v>
@@ -1245,7 +1386,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B15" s="2">
         <v>42200</v>
@@ -1258,7 +1399,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B16" s="2">
         <v>42215</v>
@@ -1271,7 +1412,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B17" s="2">
         <v>42230</v>
@@ -1284,7 +1425,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B18" s="2">
         <v>42245</v>
@@ -1297,7 +1438,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B19" s="2">
         <v>42260</v>
@@ -1310,7 +1451,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B20" s="2">
         <v>42275</v>
@@ -1323,7 +1464,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B21" s="2">
         <v>42290</v>
@@ -1336,7 +1477,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B22" s="2">
         <v>42305</v>
@@ -1349,7 +1490,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B23" s="2">
         <v>42320</v>
@@ -1362,7 +1503,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B24" s="2">
         <v>42335</v>
@@ -1375,7 +1516,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B25" s="2">
         <v>42350</v>
@@ -1388,7 +1529,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="B26" s="2">
         <v>42365</v>
@@ -1400,24 +1541,588 @@
       <c r="H26" s="2"/>
     </row>
   </sheetData>
-  <sortState ref="B3:B4">
-    <sortCondition ref="B3"/>
-  </sortState>
   <conditionalFormatting sqref="A11:A12">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B24" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>66</v>
+      </c>
+      <c r="B27" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>67</v>
+      </c>
+      <c r="B28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>68</v>
+      </c>
+      <c r="B29" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>68</v>
+      </c>
+      <c r="B30" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30" t="s">
+        <v>16</v>
+      </c>
+      <c r="D30" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>70</v>
+      </c>
+      <c r="B31" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>71</v>
+      </c>
+      <c r="B32" t="s">
+        <v>32</v>
+      </c>
+      <c r="C32" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>72</v>
+      </c>
+      <c r="B33" t="s">
+        <v>35</v>
+      </c>
+      <c r="C33" t="s">
+        <v>18</v>
+      </c>
+      <c r="D33" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>72</v>
+      </c>
+      <c r="B34" t="s">
+        <v>35</v>
+      </c>
+      <c r="C34" t="s">
+        <v>18</v>
+      </c>
+      <c r="D34" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>74</v>
+      </c>
+      <c r="B35" t="s">
+        <v>35</v>
+      </c>
+      <c r="C35" t="s">
+        <v>18</v>
+      </c>
+      <c r="D35" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>74</v>
+      </c>
+      <c r="B36" t="s">
+        <v>35</v>
+      </c>
+      <c r="C36" t="s">
+        <v>18</v>
+      </c>
+      <c r="D36" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>75</v>
+      </c>
+      <c r="B37" t="s">
+        <v>41</v>
+      </c>
+      <c r="C37" t="s">
+        <v>19</v>
+      </c>
+      <c r="D37" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>77</v>
+      </c>
+      <c r="B38" t="s">
+        <v>41</v>
+      </c>
+      <c r="C38" t="s">
+        <v>19</v>
+      </c>
+      <c r="D38" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>78</v>
+      </c>
+      <c r="B39" t="s">
+        <v>32</v>
+      </c>
+      <c r="C39" t="s">
+        <v>20</v>
+      </c>
+      <c r="D39" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>80</v>
+      </c>
+      <c r="B40" t="s">
+        <v>32</v>
+      </c>
+      <c r="C40" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" t="s">
+        <v>79</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changes made to get sprint defects based on priority
</commit_message>
<xml_diff>
--- a/examples/Defect.xlsx
+++ b/examples/Defect.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="81">
   <si>
     <t>defect ID</t>
   </si>
@@ -116,64 +116,154 @@
     <t>Sprint 25</t>
   </si>
   <si>
-    <t>January 2015</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>February 2015</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>March 2015</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>April 2015</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>May 2015</t>
-  </si>
-  <si>
-    <t>June 2015</t>
-  </si>
-  <si>
-    <t>July 2015</t>
-  </si>
-  <si>
-    <t>August 2015</t>
-  </si>
-  <si>
-    <t>September 2015</t>
-  </si>
-  <si>
-    <t>October 2015</t>
-  </si>
-  <si>
-    <t>November 2015</t>
-  </si>
-  <si>
-    <t>December 2015</t>
+    <t>2015-01-01 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-01-15 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-01-16 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-01-30 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-01-31 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-02-14 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-02-15 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-03-01 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-03-02 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-03-16 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-03-17 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-03-31 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-04-01 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-04-15 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-04-16 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-04-30 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-05-01 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-05-15 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-05-16 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-05-30 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-05-31 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-06-14 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-06-15 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-06-29 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-06-30 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-07-14 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-07-15 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-07-29 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-07-30 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-08-13 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-08-14 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-08-28 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-08-29 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-09-12 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-09-13 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-09-27 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-09-28 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-10-12 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-10-13 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-10-27 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-10-28 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-11-11 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-11-12 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-11-26 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-11-27 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-12-11 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-12-12 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-12-26 00:00:00</t>
+  </si>
+  <si>
+    <t>2015-12-27 00:00:00</t>
+  </si>
+  <si>
+    <t>2016-01-10 00:00:00</t>
   </si>
 </sst>
 </file>
@@ -212,11 +302,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -512,7 +603,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="A42" sqref="A42:C47"/>
     </sheetView>
   </sheetViews>
@@ -520,7 +611,7 @@
   <cols>
     <col min="1" max="1" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="0" style="3" hidden="1"/>
+    <col min="3" max="3" width="7.5703125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1408,219 +1499,520 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="D1" sqref="D1:D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="11.42578125" style="3"/>
+    <col min="1" max="2" width="11.42578125" style="3"/>
+    <col min="3" max="3" width="18.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
         <v>31</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>32</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="4">
+        <v>10</v>
+      </c>
+      <c r="E1" s="4">
+        <v>6</v>
+      </c>
+      <c r="F1" s="4">
+        <v>4</v>
+      </c>
+      <c r="G1" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
         <v>33</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C2" t="s">
         <v>34</v>
       </c>
-      <c r="E1" t="s">
+      <c r="D2" s="4">
+        <v>2</v>
+      </c>
+      <c r="E2" s="4">
+        <v>1</v>
+      </c>
+      <c r="F2" s="4">
+        <v>1</v>
+      </c>
+      <c r="G2" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="C3" t="s">
         <v>36</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
         <v>37</v>
       </c>
-      <c r="C2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C4" t="s">
         <v>38</v>
       </c>
-      <c r="E2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="D4" s="4">
+        <v>2</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4">
+        <v>1</v>
+      </c>
+      <c r="G4" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
         <v>39</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C5" t="s">
         <v>40</v>
       </c>
-      <c r="C3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="D5" s="4">
+        <v>3</v>
+      </c>
+      <c r="E5" s="4">
+        <v>2</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0</v>
+      </c>
+      <c r="G5" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
         <v>41</v>
       </c>
-      <c r="B4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="C6" t="s">
         <v>42</v>
       </c>
-      <c r="D4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="D6" s="4">
+        <v>1</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0</v>
+      </c>
+      <c r="G6" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
         <v>43</v>
       </c>
-      <c r="B5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="C7" t="s">
         <v>44</v>
       </c>
-      <c r="B6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="D7" s="4">
+        <v>3</v>
+      </c>
+      <c r="E7" s="4">
+        <v>2</v>
+      </c>
+      <c r="F7" s="4">
+        <v>1</v>
+      </c>
+      <c r="G7" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
         <v>45</v>
       </c>
-      <c r="B7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="C8" t="s">
         <v>46</v>
       </c>
-      <c r="B8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" t="s">
-        <v>38</v>
-      </c>
-      <c r="E8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D8" s="4">
+        <v>1</v>
+      </c>
+      <c r="E8" s="4">
+        <v>1</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0</v>
+      </c>
+      <c r="G8" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
         <v>47</v>
       </c>
-      <c r="B9" t="s">
-        <v>40</v>
-      </c>
       <c r="C9" t="s">
-        <v>40</v>
-      </c>
-      <c r="D9" t="s">
-        <v>35</v>
-      </c>
-      <c r="E9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="D9" s="4">
+        <v>2</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0</v>
+      </c>
+      <c r="F9" s="4">
+        <v>1</v>
+      </c>
+      <c r="G9" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" t="s">
-        <v>40</v>
-      </c>
-      <c r="E10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="D10" s="4">
+        <v>2</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0</v>
+      </c>
+      <c r="F10" s="4">
+        <v>1</v>
+      </c>
+      <c r="G10" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="D11" s="4">
+        <v>2</v>
+      </c>
+      <c r="E11" s="4">
+        <v>2</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0</v>
+      </c>
+      <c r="G11" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" t="s">
-        <v>35</v>
-      </c>
-      <c r="E12" t="s">
-        <v>35</v>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" s="4">
+        <v>2</v>
+      </c>
+      <c r="E14" s="4">
+        <v>1</v>
+      </c>
+      <c r="F14" s="4">
+        <v>1</v>
+      </c>
+      <c r="G14" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" s="4">
+        <v>1</v>
+      </c>
+      <c r="E15" s="4">
+        <v>1</v>
+      </c>
+      <c r="F15" s="4">
+        <v>0</v>
+      </c>
+      <c r="G15" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" t="s">
+        <v>62</v>
+      </c>
+      <c r="D16" s="4">
+        <v>3</v>
+      </c>
+      <c r="E16" s="4">
+        <v>1</v>
+      </c>
+      <c r="F16" s="4">
+        <v>1</v>
+      </c>
+      <c r="G16" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" s="4">
+        <v>2</v>
+      </c>
+      <c r="E17" s="4">
+        <v>2</v>
+      </c>
+      <c r="F17" s="4">
+        <v>0</v>
+      </c>
+      <c r="G17" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D18" s="4">
+        <v>2</v>
+      </c>
+      <c r="E18" s="4">
+        <v>2</v>
+      </c>
+      <c r="F18" s="4">
+        <v>0</v>
+      </c>
+      <c r="G18" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" t="s">
+        <v>70</v>
+      </c>
+      <c r="D20" s="4">
+        <v>4</v>
+      </c>
+      <c r="E20" s="4">
+        <v>0</v>
+      </c>
+      <c r="F20" s="4">
+        <v>4</v>
+      </c>
+      <c r="G20" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" t="s">
+        <v>73</v>
+      </c>
+      <c r="C22" t="s">
+        <v>74</v>
+      </c>
+      <c r="D22" s="4">
+        <v>2</v>
+      </c>
+      <c r="E22" s="4">
+        <v>0</v>
+      </c>
+      <c r="F22" s="4">
+        <v>0</v>
+      </c>
+      <c r="G22" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" t="s">
+        <v>75</v>
+      </c>
+      <c r="C23" t="s">
+        <v>76</v>
+      </c>
+      <c r="D23" s="4">
+        <v>1</v>
+      </c>
+      <c r="E23" s="4">
+        <v>1</v>
+      </c>
+      <c r="F23" s="4">
+        <v>0</v>
+      </c>
+      <c r="G23" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" t="s">
+        <v>77</v>
+      </c>
+      <c r="C24" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" t="s">
+        <v>79</v>
+      </c>
+      <c r="C25" t="s">
+        <v>80</v>
+      </c>
+      <c r="D25" s="4">
+        <v>1</v>
+      </c>
+      <c r="E25" s="4">
+        <v>1</v>
+      </c>
+      <c r="F25" s="4">
+        <v>0</v>
+      </c>
+      <c r="G25" s="4">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
failed attempt to count defect for each date
</commit_message>
<xml_diff>
--- a/examples/Defect.xlsx
+++ b/examples/Defect.xlsx
@@ -9,19 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Temp" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>defect ID</t>
   </si>
@@ -114,156 +114,6 @@
   </si>
   <si>
     <t>Sprint 25</t>
-  </si>
-  <si>
-    <t>2015-01-01 00:00:00</t>
-  </si>
-  <si>
-    <t>2015-01-15 00:00:00</t>
-  </si>
-  <si>
-    <t>2015-01-16 00:00:00</t>
-  </si>
-  <si>
-    <t>2015-01-30 00:00:00</t>
-  </si>
-  <si>
-    <t>2015-01-31 00:00:00</t>
-  </si>
-  <si>
-    <t>2015-02-14 00:00:00</t>
-  </si>
-  <si>
-    <t>2015-02-15 00:00:00</t>
-  </si>
-  <si>
-    <t>2015-03-01 00:00:00</t>
-  </si>
-  <si>
-    <t>2015-03-02 00:00:00</t>
-  </si>
-  <si>
-    <t>2015-03-16 00:00:00</t>
-  </si>
-  <si>
-    <t>2015-03-17 00:00:00</t>
-  </si>
-  <si>
-    <t>2015-03-31 00:00:00</t>
-  </si>
-  <si>
-    <t>2015-04-01 00:00:00</t>
-  </si>
-  <si>
-    <t>2015-04-15 00:00:00</t>
-  </si>
-  <si>
-    <t>2015-04-16 00:00:00</t>
-  </si>
-  <si>
-    <t>2015-04-30 00:00:00</t>
-  </si>
-  <si>
-    <t>2015-05-01 00:00:00</t>
-  </si>
-  <si>
-    <t>2015-05-15 00:00:00</t>
-  </si>
-  <si>
-    <t>2015-05-16 00:00:00</t>
-  </si>
-  <si>
-    <t>2015-05-30 00:00:00</t>
-  </si>
-  <si>
-    <t>2015-05-31 00:00:00</t>
-  </si>
-  <si>
-    <t>2015-06-14 00:00:00</t>
-  </si>
-  <si>
-    <t>2015-06-15 00:00:00</t>
-  </si>
-  <si>
-    <t>2015-06-29 00:00:00</t>
-  </si>
-  <si>
-    <t>2015-06-30 00:00:00</t>
-  </si>
-  <si>
-    <t>2015-07-14 00:00:00</t>
-  </si>
-  <si>
-    <t>2015-07-15 00:00:00</t>
-  </si>
-  <si>
-    <t>2015-07-29 00:00:00</t>
-  </si>
-  <si>
-    <t>2015-07-30 00:00:00</t>
-  </si>
-  <si>
-    <t>2015-08-13 00:00:00</t>
-  </si>
-  <si>
-    <t>2015-08-14 00:00:00</t>
-  </si>
-  <si>
-    <t>2015-08-28 00:00:00</t>
-  </si>
-  <si>
-    <t>2015-08-29 00:00:00</t>
-  </si>
-  <si>
-    <t>2015-09-12 00:00:00</t>
-  </si>
-  <si>
-    <t>2015-09-13 00:00:00</t>
-  </si>
-  <si>
-    <t>2015-09-27 00:00:00</t>
-  </si>
-  <si>
-    <t>2015-09-28 00:00:00</t>
-  </si>
-  <si>
-    <t>2015-10-12 00:00:00</t>
-  </si>
-  <si>
-    <t>2015-10-13 00:00:00</t>
-  </si>
-  <si>
-    <t>2015-10-27 00:00:00</t>
-  </si>
-  <si>
-    <t>2015-10-28 00:00:00</t>
-  </si>
-  <si>
-    <t>2015-11-11 00:00:00</t>
-  </si>
-  <si>
-    <t>2015-11-12 00:00:00</t>
-  </si>
-  <si>
-    <t>2015-11-26 00:00:00</t>
-  </si>
-  <si>
-    <t>2015-11-27 00:00:00</t>
-  </si>
-  <si>
-    <t>2015-12-11 00:00:00</t>
-  </si>
-  <si>
-    <t>2015-12-12 00:00:00</t>
-  </si>
-  <si>
-    <t>2015-12-26 00:00:00</t>
-  </si>
-  <si>
-    <t>2015-12-27 00:00:00</t>
-  </si>
-  <si>
-    <t>2016-01-10 00:00:00</t>
   </si>
 </sst>
 </file>
@@ -302,12 +152,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -603,8 +452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42:C47"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J51" sqref="J51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1106,7 +955,7 @@
         <v>42007</v>
       </c>
       <c r="C45">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -1117,7 +966,7 @@
         <v>42005</v>
       </c>
       <c r="C46">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -1499,523 +1348,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D25"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="11.42578125" style="3"/>
-    <col min="3" max="3" width="18.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="11.42578125" style="3"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" s="4">
-        <v>10</v>
-      </c>
-      <c r="E1" s="4">
-        <v>6</v>
-      </c>
-      <c r="F1" s="4">
-        <v>4</v>
-      </c>
-      <c r="G1" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="4">
-        <v>2</v>
-      </c>
-      <c r="E2" s="4">
-        <v>1</v>
-      </c>
-      <c r="F2" s="4">
-        <v>1</v>
-      </c>
-      <c r="G2" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" s="4">
-        <v>2</v>
-      </c>
-      <c r="E4" s="4">
-        <v>0</v>
-      </c>
-      <c r="F4" s="4">
-        <v>1</v>
-      </c>
-      <c r="G4" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" s="4">
-        <v>3</v>
-      </c>
-      <c r="E5" s="4">
-        <v>2</v>
-      </c>
-      <c r="F5" s="4">
-        <v>0</v>
-      </c>
-      <c r="G5" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" t="s">
-        <v>42</v>
-      </c>
-      <c r="D6" s="4">
-        <v>1</v>
-      </c>
-      <c r="E6" s="4">
-        <v>0</v>
-      </c>
-      <c r="F6" s="4">
-        <v>0</v>
-      </c>
-      <c r="G6" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" s="4">
-        <v>3</v>
-      </c>
-      <c r="E7" s="4">
-        <v>2</v>
-      </c>
-      <c r="F7" s="4">
-        <v>1</v>
-      </c>
-      <c r="G7" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D8" s="4">
-        <v>1</v>
-      </c>
-      <c r="E8" s="4">
-        <v>1</v>
-      </c>
-      <c r="F8" s="4">
-        <v>0</v>
-      </c>
-      <c r="G8" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" t="s">
-        <v>47</v>
-      </c>
-      <c r="C9" t="s">
-        <v>48</v>
-      </c>
-      <c r="D9" s="4">
-        <v>2</v>
-      </c>
-      <c r="E9" s="4">
-        <v>0</v>
-      </c>
-      <c r="F9" s="4">
-        <v>1</v>
-      </c>
-      <c r="G9" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C10" t="s">
-        <v>50</v>
-      </c>
-      <c r="D10" s="4">
-        <v>2</v>
-      </c>
-      <c r="E10" s="4">
-        <v>0</v>
-      </c>
-      <c r="F10" s="4">
-        <v>1</v>
-      </c>
-      <c r="G10" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" t="s">
-        <v>51</v>
-      </c>
-      <c r="C11" t="s">
-        <v>52</v>
-      </c>
-      <c r="D11" s="4">
-        <v>2</v>
-      </c>
-      <c r="E11" s="4">
-        <v>2</v>
-      </c>
-      <c r="F11" s="4">
-        <v>0</v>
-      </c>
-      <c r="G11" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" t="s">
-        <v>53</v>
-      </c>
-      <c r="C12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" t="s">
-        <v>55</v>
-      </c>
-      <c r="C13" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" t="s">
-        <v>57</v>
-      </c>
-      <c r="C14" t="s">
-        <v>58</v>
-      </c>
-      <c r="D14" s="4">
-        <v>2</v>
-      </c>
-      <c r="E14" s="4">
-        <v>1</v>
-      </c>
-      <c r="F14" s="4">
-        <v>1</v>
-      </c>
-      <c r="G14" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" t="s">
-        <v>59</v>
-      </c>
-      <c r="C15" t="s">
-        <v>60</v>
-      </c>
-      <c r="D15" s="4">
-        <v>1</v>
-      </c>
-      <c r="E15" s="4">
-        <v>1</v>
-      </c>
-      <c r="F15" s="4">
-        <v>0</v>
-      </c>
-      <c r="G15" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" t="s">
-        <v>61</v>
-      </c>
-      <c r="C16" t="s">
-        <v>62</v>
-      </c>
-      <c r="D16" s="4">
-        <v>3</v>
-      </c>
-      <c r="E16" s="4">
-        <v>1</v>
-      </c>
-      <c r="F16" s="4">
-        <v>1</v>
-      </c>
-      <c r="G16" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" t="s">
-        <v>63</v>
-      </c>
-      <c r="C17" t="s">
-        <v>64</v>
-      </c>
-      <c r="D17" s="4">
-        <v>2</v>
-      </c>
-      <c r="E17" s="4">
-        <v>2</v>
-      </c>
-      <c r="F17" s="4">
-        <v>0</v>
-      </c>
-      <c r="G17" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" t="s">
-        <v>65</v>
-      </c>
-      <c r="C18" t="s">
-        <v>66</v>
-      </c>
-      <c r="D18" s="4">
-        <v>2</v>
-      </c>
-      <c r="E18" s="4">
-        <v>2</v>
-      </c>
-      <c r="F18" s="4">
-        <v>0</v>
-      </c>
-      <c r="G18" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" t="s">
-        <v>67</v>
-      </c>
-      <c r="C19" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20" t="s">
-        <v>69</v>
-      </c>
-      <c r="C20" t="s">
-        <v>70</v>
-      </c>
-      <c r="D20" s="4">
-        <v>4</v>
-      </c>
-      <c r="E20" s="4">
-        <v>0</v>
-      </c>
-      <c r="F20" s="4">
-        <v>4</v>
-      </c>
-      <c r="G20" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21" t="s">
-        <v>71</v>
-      </c>
-      <c r="C21" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>27</v>
-      </c>
-      <c r="B22" t="s">
-        <v>73</v>
-      </c>
-      <c r="C22" t="s">
-        <v>74</v>
-      </c>
-      <c r="D22" s="4">
-        <v>2</v>
-      </c>
-      <c r="E22" s="4">
-        <v>0</v>
-      </c>
-      <c r="F22" s="4">
-        <v>0</v>
-      </c>
-      <c r="G22" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>28</v>
-      </c>
-      <c r="B23" t="s">
-        <v>75</v>
-      </c>
-      <c r="C23" t="s">
-        <v>76</v>
-      </c>
-      <c r="D23" s="4">
-        <v>1</v>
-      </c>
-      <c r="E23" s="4">
-        <v>1</v>
-      </c>
-      <c r="F23" s="4">
-        <v>0</v>
-      </c>
-      <c r="G23" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>29</v>
-      </c>
-      <c r="B24" t="s">
-        <v>77</v>
-      </c>
-      <c r="C24" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>30</v>
-      </c>
-      <c r="B25" t="s">
-        <v>79</v>
-      </c>
-      <c r="C25" t="s">
-        <v>80</v>
-      </c>
-      <c r="D25" s="4">
-        <v>1</v>
-      </c>
-      <c r="E25" s="4">
-        <v>1</v>
-      </c>
-      <c r="F25" s="4">
-        <v>0</v>
-      </c>
-      <c r="G25" s="4">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>